<commit_message>
Added to Matt's script. Found individual samples that contain both RNA/ChRO-seq
</commit_message>
<xml_diff>
--- a/FLC/Sample Log/FLC_mito_data.xlsx
+++ b/FLC/Sample Log/FLC_mito_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arfantastic/Git/SethupathyLab/FLC/Sample Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC196A87-543B-2743-9FDF-2C746AF770C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC9EA58-AC76-9841-A872-9D89AE56EC1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5F9A7AC4-3AA5-9046-9F70-89C2642F0525}"/>
   </bookViews>
@@ -1267,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE19CBB1-0CE0-9F44-98D2-8CBDE065BB56}">
   <dimension ref="A1:AU115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
I found some samples that were not probably labeled in the primary sample log (FLC09_TZOG, FLC26_ICBQ, FLC27_XDGP). These were updated and the script was run again.
</commit_message>
<xml_diff>
--- a/FLC/Sample Log/FLC_mito_data.xlsx
+++ b/FLC/Sample Log/FLC_mito_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arfantastic/Git/SethupathyLab/FLC/Sample Log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC9EA58-AC76-9841-A872-9D89AE56EC1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B4847-5966-F441-BEBC-2D2330A4E529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5F9A7AC4-3AA5-9046-9F70-89C2642F0525}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
   <dimension ref="A1:AU115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>